<commit_message>
finally created fileutils to better handle io
</commit_message>
<xml_diff>
--- a/src/main/resources/java-developer-philly-rubric-template.xlsx
+++ b/src/main/resources/java-developer-philly-rubric-template.xlsx
@@ -2,6 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
   <sheets>
     <sheet state="visible" name="Main" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Project Management Methodologie" sheetId="2" r:id="rId5"/>
@@ -170,6 +173,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="0"/>
   <fonts count="19">
     <font>
       <sz val="10.0"/>
@@ -767,6 +771,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:L916"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2.0" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -775,17 +780,17 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="24.14"/>
-    <col customWidth="1" min="2" max="2" width="11.43"/>
-    <col customWidth="1" min="3" max="3" width="39.29"/>
-    <col customWidth="1" min="4" max="4" width="19.29"/>
-    <col customWidth="1" min="5" max="5" width="38.71"/>
-    <col customWidth="1" min="6" max="6" width="23.0"/>
-    <col customWidth="1" min="7" max="7" width="8.29"/>
-    <col customWidth="1" min="8" max="8" width="16.57"/>
-    <col customWidth="1" min="9" max="10" width="30.14"/>
-    <col customWidth="1" min="11" max="11" width="26.57"/>
-    <col customWidth="1" min="12" max="12" width="41.57"/>
+    <col min="1" max="1" customWidth="true" width="24.14" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.43" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="39.29" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="19.29" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="38.71" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="8.29" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.57" collapsed="true"/>
+    <col min="9" max="10" customWidth="true" width="30.14" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="26.57" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="41.57" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="39.75" customHeight="1">
@@ -14309,15 +14314,16 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D977"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="17.86"/>
-    <col customWidth="1" min="2" max="2" width="18.29"/>
-    <col customWidth="1" min="3" max="3" width="31.57"/>
-    <col customWidth="1" min="4" max="4" width="23.0"/>
+    <col min="1" max="1" customWidth="true" width="17.86" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.29" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="31.57" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="40.5" customHeight="1">
@@ -16546,14 +16552,15 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:E979"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="17.86"/>
-    <col customWidth="1" min="2" max="2" width="18.29"/>
-    <col customWidth="1" min="3" max="5" width="26.29"/>
+    <col min="1" max="1" customWidth="true" width="17.86" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.29" collapsed="true"/>
+    <col min="3" max="5" customWidth="true" width="26.29" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="40.5" customHeight="1">
@@ -19042,14 +19049,15 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:E970"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="17.86"/>
-    <col customWidth="1" min="2" max="2" width="18.29"/>
-    <col customWidth="1" min="3" max="5" width="26.29"/>
+    <col min="1" max="1" customWidth="true" width="17.86" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.29" collapsed="true"/>
+    <col min="3" max="5" customWidth="true" width="26.29" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="40.5" customHeight="1">
@@ -21467,15 +21475,16 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D974"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="17.86"/>
-    <col customWidth="1" min="2" max="2" width="18.29"/>
-    <col customWidth="1" min="3" max="3" width="34.43"/>
-    <col customWidth="1" min="4" max="4" width="27.14"/>
+    <col min="1" max="1" customWidth="true" width="17.86" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.29" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="34.43" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.14" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="40.5" customHeight="1">
@@ -23604,6 +23613,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -23865,6 +23875,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -24103,6 +24114,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -24360,6 +24372,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>

</xml_diff>